<commit_message>
exploring if, ifs, and, or functions
</commit_message>
<xml_diff>
--- a/logical_functions.xlsx
+++ b/logical_functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walka\MyGit\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A41D3F-2D60-440B-9500-FF29C5D61B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E3E62E-3B2A-486B-A358-4DAF6D5C1BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{62628B09-4AB9-4541-A249-672E054863C4}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="Final_2" sheetId="7" r:id="rId4"/>
     <sheet name="Errors" sheetId="4" r:id="rId5"/>
     <sheet name="And-Or" sheetId="5" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="145">
   <si>
     <t>Job Title</t>
   </si>
@@ -494,6 +493,9 @@
   </si>
   <si>
     <t>Condition 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -504,7 +506,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,8 +556,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,6 +590,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -831,11 +857,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -886,7 +914,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -921,8 +948,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1236,10 +1267,724 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5EA319-2E76-4900-9BC8-0F42AC70BCA5}">
+  <dimension ref="B1:R16"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="12.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="19.21875" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.77734375" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10.77734375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.21875" style="1"/>
+    <col min="18" max="18" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="2:18" s="10" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2"/>
+      <c r="R2"/>
+    </row>
+    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12">
+        <v>120000</v>
+      </c>
+      <c r="E3" s="13">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="14">
+        <f>C3</f>
+        <v>5</v>
+      </c>
+      <c r="G3" s="15">
+        <f>D3+E3</f>
+        <v>130000</v>
+      </c>
+      <c r="H3" s="16">
+        <f>E3/D3</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I3" s="17">
+        <f>D3+D3*H3</f>
+        <v>130000</v>
+      </c>
+      <c r="J3" s="15" t="b">
+        <f>G3=I3</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="15" t="b">
+        <f>E3&gt;D3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="15" t="b">
+        <f t="shared" ref="L3:L12" si="0">$C$15&lt;=C3</f>
+        <v>1</v>
+      </c>
+      <c r="M3" s="15" t="b">
+        <f t="shared" ref="M3:M12" si="1">$G3&gt;=$C$16</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="15">
+        <f>L3*M3</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="15" t="b">
+        <f>L3*M3=1</f>
+        <v>1</v>
+      </c>
+      <c r="P3" s="15" t="b">
+        <f>AND(L3,M3)</f>
+        <v>1</v>
+      </c>
+      <c r="Q3"/>
+      <c r="R3"/>
+    </row>
+    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="12">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12">
+        <v>135000</v>
+      </c>
+      <c r="E4" s="13">
+        <v>12000</v>
+      </c>
+      <c r="F4" s="14">
+        <f t="shared" ref="F4:F12" si="2">C4</f>
+        <v>4</v>
+      </c>
+      <c r="G4" s="15">
+        <f t="shared" ref="G4:G12" si="3">D4+E4</f>
+        <v>147000</v>
+      </c>
+      <c r="H4" s="16">
+        <f t="shared" ref="H4:H12" si="4">E4/D4</f>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="I4" s="17">
+        <f t="shared" ref="I4:I12" si="5">D4+D4*H4</f>
+        <v>147000</v>
+      </c>
+      <c r="J4" s="15" t="b">
+        <f t="shared" ref="J4:J12" si="6">G4=I4</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="15" t="b">
+        <f t="shared" ref="K4:K12" si="7">E4&gt;D4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N4" s="15">
+        <f t="shared" ref="N4:N12" si="8">L4*M4</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="15" t="b">
+        <f t="shared" ref="O4:O12" si="9">L4*M4=1</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="15" t="b">
+        <f t="shared" ref="P4:P12" si="10">AND(L4,M4)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4"/>
+      <c r="R4"/>
+    </row>
+    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2</v>
+      </c>
+      <c r="D5" s="12">
+        <v>75000</v>
+      </c>
+      <c r="E5" s="13">
+        <v>5000</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G5" s="15">
+        <f t="shared" si="3"/>
+        <v>80000</v>
+      </c>
+      <c r="H5" s="16">
+        <f t="shared" si="4"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I5" s="17">
+        <f t="shared" si="5"/>
+        <v>80000</v>
+      </c>
+      <c r="J5" s="15" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="15" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="15" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="15" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="15" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q5"/>
+      <c r="R5"/>
+    </row>
+    <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="12">
+        <v>6</v>
+      </c>
+      <c r="D6" s="12">
+        <v>110000</v>
+      </c>
+      <c r="E6" s="13">
+        <v>8000</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G6" s="15">
+        <f t="shared" si="3"/>
+        <v>118000</v>
+      </c>
+      <c r="H6" s="16">
+        <f t="shared" si="4"/>
+        <v>7.2727272727272724E-2</v>
+      </c>
+      <c r="I6" s="17">
+        <f t="shared" si="5"/>
+        <v>118000</v>
+      </c>
+      <c r="J6" s="15" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="15" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M6" s="15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N6" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="15" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P6" s="15" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="Q6"/>
+      <c r="R6"/>
+    </row>
+    <row r="7" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="12">
+        <v>3</v>
+      </c>
+      <c r="D7" s="12">
+        <v>125000</v>
+      </c>
+      <c r="E7" s="13">
+        <v>11000</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G7" s="15">
+        <f t="shared" si="3"/>
+        <v>136000</v>
+      </c>
+      <c r="H7" s="16">
+        <f t="shared" si="4"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I7" s="17">
+        <f t="shared" si="5"/>
+        <v>136000</v>
+      </c>
+      <c r="J7" s="15" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="15" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N7" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="15" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="15" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q7"/>
+      <c r="R7"/>
+    </row>
+    <row r="8" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="12">
+        <v>7</v>
+      </c>
+      <c r="D8" s="12">
+        <v>90000</v>
+      </c>
+      <c r="E8" s="13">
+        <v>7000</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G8" s="15">
+        <f t="shared" si="3"/>
+        <v>97000</v>
+      </c>
+      <c r="H8" s="16">
+        <f t="shared" si="4"/>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="I8" s="17">
+        <f t="shared" si="5"/>
+        <v>97000</v>
+      </c>
+      <c r="J8" s="15" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="15" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M8" s="15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N8" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O8" s="15" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P8" s="15" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="Q8"/>
+      <c r="R8"/>
+    </row>
+    <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="12">
+        <v>10</v>
+      </c>
+      <c r="D9" s="12">
+        <v>150000</v>
+      </c>
+      <c r="E9" s="13">
+        <v>15000</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G9" s="15">
+        <f t="shared" si="3"/>
+        <v>165000</v>
+      </c>
+      <c r="H9" s="16">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="17">
+        <f t="shared" si="5"/>
+        <v>165000</v>
+      </c>
+      <c r="J9" s="15" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="15" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O9" s="15" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P9" s="15" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="Q9"/>
+      <c r="R9"/>
+    </row>
+    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="12">
+        <v>8</v>
+      </c>
+      <c r="D10" s="12">
+        <v>130000</v>
+      </c>
+      <c r="E10" s="13">
+        <v>13000</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G10" s="15">
+        <f t="shared" si="3"/>
+        <v>143000</v>
+      </c>
+      <c r="H10" s="16">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="17">
+        <f t="shared" si="5"/>
+        <v>143000</v>
+      </c>
+      <c r="J10" s="15" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="15" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M10" s="15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N10" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O10" s="15" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P10" s="15" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="Q10"/>
+      <c r="R10"/>
+    </row>
+    <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="12">
+        <v>3</v>
+      </c>
+      <c r="D11" s="12">
+        <v>140000</v>
+      </c>
+      <c r="E11" s="13">
+        <v>14000</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G11" s="15">
+        <f t="shared" si="3"/>
+        <v>154000</v>
+      </c>
+      <c r="H11" s="16">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="17">
+        <f t="shared" si="5"/>
+        <v>154000</v>
+      </c>
+      <c r="J11" s="15" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="15" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N11" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="15" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="15" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q11"/>
+      <c r="R11"/>
+    </row>
+    <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="20">
+        <v>5</v>
+      </c>
+      <c r="D12" s="20">
+        <v>115000</v>
+      </c>
+      <c r="E12" s="21">
+        <v>9000</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G12" s="15">
+        <f t="shared" si="3"/>
+        <v>124000</v>
+      </c>
+      <c r="H12" s="16">
+        <f t="shared" si="4"/>
+        <v>7.8260869565217397E-2</v>
+      </c>
+      <c r="I12" s="17">
+        <f t="shared" si="5"/>
+        <v>124000</v>
+      </c>
+      <c r="J12" s="15" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="15" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M12" s="15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="15" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P12" s="15" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="Q12"/>
+      <c r="R12"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="Q13"/>
+      <c r="R13"/>
+    </row>
+    <row r="14" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q14"/>
+      <c r="R14"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="26">
+        <v>90000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FB8CF7-38C1-4709-B7C6-4142FE426970}">
   <dimension ref="B1:Q16"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1374,7 +2119,10 @@
         <f>AND(L3,M3)</f>
         <v>1</v>
       </c>
-      <c r="Q3" s="18"/>
+      <c r="Q3" s="18" t="str">
+        <f>IF(P3, "Goal Met", "Not Met")</f>
+        <v>Goal Met</v>
+      </c>
     </row>
     <row r="4" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
@@ -1433,7 +2181,10 @@
         <f t="shared" ref="P4:P12" si="10">AND(L4,M4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="18"/>
+      <c r="Q4" s="18" t="str">
+        <f t="shared" ref="Q4:Q12" si="11">IF(P4, "Goal Met", "Not Met")</f>
+        <v>Not Met</v>
+      </c>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
@@ -1492,7 +2243,10 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q5" s="18"/>
+      <c r="Q5" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>Not Met</v>
+      </c>
     </row>
     <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
@@ -1551,7 +2305,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q6" s="18"/>
+      <c r="Q6" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
     </row>
     <row r="7" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="11" t="s">
@@ -1610,7 +2367,10 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="18"/>
+      <c r="Q7" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>Not Met</v>
+      </c>
     </row>
     <row r="8" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
@@ -1669,7 +2429,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q8" s="18"/>
+      <c r="Q8" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
     </row>
     <row r="9" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
@@ -1728,7 +2491,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q9" s="18"/>
+      <c r="Q9" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
     </row>
     <row r="10" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
@@ -1787,7 +2553,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="18"/>
+      <c r="Q10" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
     </row>
     <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
@@ -1846,7 +2615,10 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="18"/>
+      <c r="Q11" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>Not Met</v>
+      </c>
     </row>
     <row r="12" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="19" t="s">
@@ -1905,725 +2677,29 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q12" s="22"/>
+      <c r="Q12" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
     </row>
     <row r="14" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="24">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="27">
-        <v>90000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FB8CF7-38C1-4709-B7C6-4142FE426970}">
-  <dimension ref="B1:Q16"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="12.44140625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="19.21875" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.21875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.77734375" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="10.77734375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.21875" style="1"/>
-    <col min="18" max="18" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="2:17" s="10" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="12">
-        <v>5</v>
-      </c>
-      <c r="D3" s="12">
-        <v>120000</v>
-      </c>
-      <c r="E3" s="13">
-        <v>10000</v>
-      </c>
-      <c r="F3" s="14">
-        <f>C3</f>
-        <v>5</v>
-      </c>
-      <c r="G3" s="15">
-        <f>D3+E3</f>
-        <v>130000</v>
-      </c>
-      <c r="H3" s="16">
-        <f>E3/D3</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="I3" s="17">
-        <f>D3+D3*H3</f>
-        <v>130000</v>
-      </c>
-      <c r="J3" s="15" t="b">
-        <f>G3=I3</f>
-        <v>1</v>
-      </c>
-      <c r="K3" s="15" t="b">
-        <f>E3&gt;D3</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="15" t="b">
-        <f t="shared" ref="L3:L12" si="0">$C$15&lt;=C3</f>
-        <v>1</v>
-      </c>
-      <c r="M3" s="15" t="b">
-        <f t="shared" ref="M3:M12" si="1">$G3&gt;=$C$16</f>
-        <v>1</v>
-      </c>
-      <c r="N3" s="15">
-        <f>L3*M3</f>
-        <v>1</v>
-      </c>
-      <c r="O3" s="15" t="b">
-        <f>L3*M3=1</f>
-        <v>1</v>
-      </c>
-      <c r="P3" s="15" t="b">
-        <f>AND(L3,M3)</f>
-        <v>1</v>
-      </c>
-      <c r="Q3" s="18"/>
-    </row>
-    <row r="4" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="12">
-        <v>4</v>
-      </c>
-      <c r="D4" s="12">
-        <v>135000</v>
-      </c>
-      <c r="E4" s="13">
-        <v>12000</v>
-      </c>
-      <c r="F4" s="14">
-        <f t="shared" ref="F4:F12" si="2">C4</f>
-        <v>4</v>
-      </c>
-      <c r="G4" s="15">
-        <f t="shared" ref="G4:G12" si="3">D4+E4</f>
-        <v>147000</v>
-      </c>
-      <c r="H4" s="16">
-        <f t="shared" ref="H4:H12" si="4">E4/D4</f>
-        <v>8.8888888888888892E-2</v>
-      </c>
-      <c r="I4" s="17">
-        <f t="shared" ref="I4:I12" si="5">D4+D4*H4</f>
-        <v>147000</v>
-      </c>
-      <c r="J4" s="15" t="b">
-        <f t="shared" ref="J4:J12" si="6">G4=I4</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="15" t="b">
-        <f t="shared" ref="K4:K12" si="7">E4&gt;D4</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="15" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M4" s="15" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N4" s="15">
-        <f t="shared" ref="N4:N12" si="8">L4*M4</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="15" t="b">
-        <f t="shared" ref="O4:O12" si="9">L4*M4=1</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="15" t="b">
-        <f t="shared" ref="P4:P12" si="10">AND(L4,M4)</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="18"/>
-    </row>
-    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="12">
-        <v>2</v>
-      </c>
-      <c r="D5" s="12">
-        <v>75000</v>
-      </c>
-      <c r="E5" s="13">
-        <v>5000</v>
-      </c>
-      <c r="F5" s="14">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="G5" s="15">
-        <f t="shared" si="3"/>
-        <v>80000</v>
-      </c>
-      <c r="H5" s="16">
-        <f t="shared" si="4"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="I5" s="17">
-        <f t="shared" si="5"/>
-        <v>80000</v>
-      </c>
-      <c r="J5" s="15" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K5" s="15" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="15" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="15" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="15" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="15" t="b">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="18"/>
-    </row>
-    <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="12">
-        <v>6</v>
-      </c>
-      <c r="D6" s="12">
-        <v>110000</v>
-      </c>
-      <c r="E6" s="13">
-        <v>8000</v>
-      </c>
-      <c r="F6" s="14">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="G6" s="15">
-        <f t="shared" si="3"/>
-        <v>118000</v>
-      </c>
-      <c r="H6" s="16">
-        <f t="shared" si="4"/>
-        <v>7.2727272727272724E-2</v>
-      </c>
-      <c r="I6" s="17">
-        <f t="shared" si="5"/>
-        <v>118000</v>
-      </c>
-      <c r="J6" s="15" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K6" s="15" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L6" s="15" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M6" s="15" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N6" s="15">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O6" s="15" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P6" s="15" t="b">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="Q6" s="18"/>
-    </row>
-    <row r="7" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="12">
-        <v>3</v>
-      </c>
-      <c r="D7" s="12">
-        <v>125000</v>
-      </c>
-      <c r="E7" s="13">
-        <v>11000</v>
-      </c>
-      <c r="F7" s="14">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="G7" s="15">
-        <f t="shared" si="3"/>
-        <v>136000</v>
-      </c>
-      <c r="H7" s="16">
-        <f t="shared" si="4"/>
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="I7" s="17">
-        <f t="shared" si="5"/>
-        <v>136000</v>
-      </c>
-      <c r="J7" s="15" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K7" s="15" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="15" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="15" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N7" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="15" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="15" t="b">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="18"/>
-    </row>
-    <row r="8" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="12">
-        <v>7</v>
-      </c>
-      <c r="D8" s="12">
-        <v>90000</v>
-      </c>
-      <c r="E8" s="13">
-        <v>7000</v>
-      </c>
-      <c r="F8" s="14">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="G8" s="15">
-        <f t="shared" si="3"/>
-        <v>97000</v>
-      </c>
-      <c r="H8" s="16">
-        <f t="shared" si="4"/>
-        <v>7.7777777777777779E-2</v>
-      </c>
-      <c r="I8" s="17">
-        <f t="shared" si="5"/>
-        <v>97000</v>
-      </c>
-      <c r="J8" s="15" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K8" s="15" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="15" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M8" s="15" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N8" s="15">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O8" s="15" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P8" s="15" t="b">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="Q8" s="18"/>
-    </row>
-    <row r="9" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="12">
-        <v>10</v>
-      </c>
-      <c r="D9" s="12">
-        <v>150000</v>
-      </c>
-      <c r="E9" s="13">
-        <v>15000</v>
-      </c>
-      <c r="F9" s="14">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="G9" s="15">
-        <f t="shared" si="3"/>
-        <v>165000</v>
-      </c>
-      <c r="H9" s="16">
-        <f t="shared" si="4"/>
-        <v>0.1</v>
-      </c>
-      <c r="I9" s="17">
-        <f t="shared" si="5"/>
-        <v>165000</v>
-      </c>
-      <c r="J9" s="15" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K9" s="15" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="15" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M9" s="15" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N9" s="15">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O9" s="15" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P9" s="15" t="b">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="Q9" s="18"/>
-    </row>
-    <row r="10" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="12">
-        <v>8</v>
-      </c>
-      <c r="D10" s="12">
-        <v>130000</v>
-      </c>
-      <c r="E10" s="13">
-        <v>13000</v>
-      </c>
-      <c r="F10" s="14">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="G10" s="15">
-        <f t="shared" si="3"/>
-        <v>143000</v>
-      </c>
-      <c r="H10" s="16">
-        <f t="shared" si="4"/>
-        <v>0.1</v>
-      </c>
-      <c r="I10" s="17">
-        <f t="shared" si="5"/>
-        <v>143000</v>
-      </c>
-      <c r="J10" s="15" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K10" s="15" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="15" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M10" s="15" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N10" s="15">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O10" s="15" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P10" s="15" t="b">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="Q10" s="18"/>
-    </row>
-    <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="12">
-        <v>3</v>
-      </c>
-      <c r="D11" s="12">
-        <v>140000</v>
-      </c>
-      <c r="E11" s="13">
-        <v>14000</v>
-      </c>
-      <c r="F11" s="14">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="G11" s="15">
-        <f t="shared" si="3"/>
-        <v>154000</v>
-      </c>
-      <c r="H11" s="16">
-        <f t="shared" si="4"/>
-        <v>0.1</v>
-      </c>
-      <c r="I11" s="17">
-        <f t="shared" si="5"/>
-        <v>154000</v>
-      </c>
-      <c r="J11" s="15" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K11" s="15" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="15" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="15" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N11" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="15" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="15" t="b">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="18"/>
-    </row>
-    <row r="12" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="20">
-        <v>5</v>
-      </c>
-      <c r="D12" s="20">
-        <v>115000</v>
-      </c>
-      <c r="E12" s="21">
-        <v>9000</v>
-      </c>
-      <c r="F12" s="14">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="G12" s="15">
-        <f t="shared" si="3"/>
-        <v>124000</v>
-      </c>
-      <c r="H12" s="16">
-        <f t="shared" si="4"/>
-        <v>7.8260869565217397E-2</v>
-      </c>
-      <c r="I12" s="17">
-        <f t="shared" si="5"/>
-        <v>124000</v>
-      </c>
-      <c r="J12" s="15" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K12" s="15" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="15" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M12" s="15" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N12" s="15">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O12" s="15" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P12" s="15" t="b">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="Q12" s="22"/>
-    </row>
-    <row r="14" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="27">
+      <c r="C16" s="26">
         <v>90000</v>
       </c>
     </row>
@@ -2637,708 +2713,705 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="O20" sqref="O19:P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="75.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1"/>
     <col min="12" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" customWidth="1"/>
     <col min="18" max="18" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1" s="31" t="s">
+      <c r="I1" s="30"/>
+      <c r="J1" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="Q1" s="30">
+      <c r="Q1" s="29">
         <v>85000</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="R1" s="29" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="28">
         <v>44996.547291666669</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="27">
         <v>135000</v>
       </c>
-      <c r="I2" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="28" t="s">
+      <c r="I2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="27" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="28">
         <v>45097.915243055562</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="27">
         <v>35000</v>
       </c>
-      <c r="I3" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="28" t="s">
+      <c r="I3" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="27" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="28">
         <v>45173.250416666669</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="28" t="s">
+      <c r="H4" s="27"/>
+      <c r="I4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="28">
         <v>45156.253321759257</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="28" t="s">
+      <c r="H5" s="27"/>
+      <c r="I5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="27" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="28">
         <v>45147.802951388891</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="28" t="s">
+      <c r="H6" s="27"/>
+      <c r="I6" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="28">
         <v>45202.753101851849</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="28" t="s">
+      <c r="H7" s="27"/>
+      <c r="I7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="28">
         <v>44949.850462962961</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="28" t="s">
+      <c r="H8" s="27"/>
+      <c r="I8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="27" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="28">
         <v>45001.627175925933</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="27">
         <v>115000</v>
       </c>
-      <c r="I9" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="28" t="s">
+      <c r="I9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="28">
         <v>45041.375868055547</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="28" t="s">
+      <c r="H10" s="27"/>
+      <c r="I10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="27" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="28">
         <v>45106.587094907409</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="27">
         <v>105000</v>
       </c>
-      <c r="I11" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="28" t="s">
+      <c r="I11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="28">
         <v>45029.919687499998</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="27">
         <v>195000</v>
       </c>
-      <c r="I12" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="28" t="s">
+      <c r="I12" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="28">
         <v>45091.502789351849</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="27">
         <v>165000</v>
       </c>
-      <c r="I13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="28" t="s">
+      <c r="I13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="28">
         <v>45175.543124999997</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="27">
         <v>281450.5</v>
       </c>
-      <c r="I14" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="28" t="s">
+      <c r="I14" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="28">
         <v>45117.778391203698</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="27">
         <v>70000</v>
       </c>
-      <c r="I15" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="28" t="s">
+      <c r="I15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="27" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="28">
         <v>44938.614351851851</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="27">
         <v>98301.5</v>
       </c>
-      <c r="I16" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="28" t="s">
+      <c r="I16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="28">
         <v>44985.354097222233</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="27">
         <v>89100</v>
       </c>
-      <c r="I17" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="28" t="s">
+      <c r="I17" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="28">
         <v>45063.792291666658</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="G18" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" s="28" t="s">
+      <c r="H18" s="27"/>
+      <c r="I18" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="28">
         <v>45017.004837962973</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="28" t="s">
+      <c r="G19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H19" s="27">
         <v>87500</v>
       </c>
-      <c r="I19" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="28" t="s">
+      <c r="I19" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="28">
         <v>45169.64203703704</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="G20" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" s="28" t="s">
+      <c r="H20" s="27"/>
+      <c r="I20" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" s="27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="28">
         <v>45000.542685185188</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21" s="27">
         <v>90000</v>
       </c>
-      <c r="I21" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="28" t="s">
+      <c r="I21" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="27" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3352,709 +3425,1349 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="42.44140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="75.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="75.77734375" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.77734375" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" customWidth="1"/>
+    <col min="16" max="16" width="13.77734375" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="Q1" s="30">
+      <c r="Q1" s="29">
         <v>85000</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="R1" s="29" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="28">
         <v>44996.547291666669</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="27">
         <v>135000</v>
       </c>
-      <c r="I2" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="28" t="s">
+      <c r="I2" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="27" t="s">
         <v>105</v>
       </c>
+      <c r="K2" t="str">
+        <f>IF($A2=K$1, "Role Desired", "Not Desired")</f>
+        <v>Not Desired</v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF($A2=L$1, "Role Desired", "Not Desired")</f>
+        <v>Not Desired</v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF($A2=K$1, "Role Desired", IF($A2=L$1, "Role Desired", "Not Desired"))</f>
+        <v>Not Desired</v>
+      </c>
+      <c r="N2" t="b">
+        <f>AND($A2=K$1, $A2=L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <f>OR($A2=K$1, $A2=L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" t="str">
+        <f>IF(OR($A2=K$1, $A2=L$1), "Role Desired", "Not Desired")</f>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>IF($H2&gt;Q$1, "Salary &gt; 85K", "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
+      </c>
+      <c r="R2" t="str" cm="1">
+        <f t="array" ref="R2">_xlfn.IFS($H2="", "No Data", $H2&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="28">
         <v>45097.915243055562</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="27">
         <v>35000</v>
       </c>
-      <c r="I3" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="28" t="s">
+      <c r="I3" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="27" t="s">
         <v>101</v>
       </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:L21" si="0">IF($A3=K$1, "Role Desired", "Not Desired")</f>
+        <v>Role Desired</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M21" si="1">IF($A3=K$1, "Role Desired", IF($A3=L$1, "Role Desired", "Not Desired"))</f>
+        <v>Role Desired</v>
+      </c>
+      <c r="N3" t="b">
+        <f t="shared" ref="N3:N21" si="2">AND($A3=K$1, $A3=L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <f t="shared" ref="O3:O21" si="3">OR($A3=K$1, $A3=L$1)</f>
+        <v>1</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P21" si="4">IF(OR($A3=K$1, $A3=L$1), "Role Desired", "Not Desired")</f>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q21" si="5">IF($H3&gt;Q$1, "Salary &gt; 85K", "Salary Low")</f>
+        <v>Salary Low</v>
+      </c>
+      <c r="R3" t="str" cm="1">
+        <f t="array" ref="R3">_xlfn.IFS($H3="", "No Data", $H3&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary Low</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="28">
         <v>45173.250416666669</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="28" t="s">
+      <c r="H4" s="27"/>
+      <c r="I4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="27" t="s">
         <v>98</v>
       </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q4" s="44" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary Low</v>
+      </c>
+      <c r="R4" s="45" t="str" cm="1">
+        <f t="array" ref="R4">_xlfn.IFS($H4="", "No Data", $H4&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="28">
         <v>45156.253321759257</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="28" t="s">
+      <c r="H5" s="27"/>
+      <c r="I5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="27" t="s">
         <v>95</v>
       </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N5" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q5" s="44" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary Low</v>
+      </c>
+      <c r="R5" s="45" t="str" cm="1">
+        <f t="array" ref="R5">_xlfn.IFS($H5="", "No Data", $H5&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="28">
         <v>45147.802951388891</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="28" t="s">
+      <c r="H6" s="27"/>
+      <c r="I6" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="27" t="s">
         <v>91</v>
       </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N6" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O6" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q6" s="44" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary Low</v>
+      </c>
+      <c r="R6" s="45" t="str" cm="1">
+        <f t="array" ref="R6">_xlfn.IFS($H6="", "No Data", $H6&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="28">
         <v>45202.753101851849</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="28" t="s">
+      <c r="H7" s="27"/>
+      <c r="I7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="27" t="s">
         <v>86</v>
       </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N7" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q7" s="44" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary Low</v>
+      </c>
+      <c r="R7" s="45" t="str" cm="1">
+        <f t="array" ref="R7">_xlfn.IFS($H7="", "No Data", $H7&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="28">
         <v>44949.850462962961</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="28" t="s">
+      <c r="H8" s="27"/>
+      <c r="I8" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="27" t="s">
         <v>83</v>
       </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N8" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q8" s="44" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary Low</v>
+      </c>
+      <c r="R8" s="45" t="str" cm="1">
+        <f t="array" ref="R8">_xlfn.IFS($H8="", "No Data", $H8&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="28">
         <v>45001.627175925933</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="27">
         <v>115000</v>
       </c>
-      <c r="I9" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="28" t="s">
+      <c r="I9" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="27" t="s">
         <v>80</v>
       </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N9" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O9" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary &gt; 85K</v>
+      </c>
+      <c r="R9" t="str" cm="1">
+        <f t="array" ref="R9">_xlfn.IFS($H9="", "No Data", $H9&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="28">
         <v>45041.375868055547</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="28" t="s">
+      <c r="H10" s="27"/>
+      <c r="I10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="27" t="s">
         <v>76</v>
       </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N10" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O10" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q10" s="44" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary Low</v>
+      </c>
+      <c r="R10" s="45" t="str" cm="1">
+        <f t="array" ref="R10">_xlfn.IFS($H10="", "No Data", $H10&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="28">
         <v>45106.587094907409</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="27">
         <v>105000</v>
       </c>
-      <c r="I11" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="28" t="s">
+      <c r="I11" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="27" t="s">
         <v>73</v>
       </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N11" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O11" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary &gt; 85K</v>
+      </c>
+      <c r="R11" t="str" cm="1">
+        <f t="array" ref="R11">_xlfn.IFS($H11="", "No Data", $H11&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="28">
         <v>45029.919687499998</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="27">
         <v>195000</v>
       </c>
-      <c r="I12" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="28" t="s">
+      <c r="I12" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="27" t="s">
         <v>70</v>
       </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N12" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O12" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary &gt; 85K</v>
+      </c>
+      <c r="R12" t="str" cm="1">
+        <f t="array" ref="R12">_xlfn.IFS($H12="", "No Data", $H12&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="28">
         <v>45091.502789351849</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="27">
         <v>165000</v>
       </c>
-      <c r="I13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="28" t="s">
+      <c r="I13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="27" t="s">
         <v>66</v>
       </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N13" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O13" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary &gt; 85K</v>
+      </c>
+      <c r="R13" t="str" cm="1">
+        <f t="array" ref="R13">_xlfn.IFS($H13="", "No Data", $H13&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="28">
         <v>45175.543124999997</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="27">
         <v>281450.5</v>
       </c>
-      <c r="I14" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="28" t="s">
+      <c r="I14" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="27" t="s">
         <v>62</v>
       </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N14" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O14" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary &gt; 85K</v>
+      </c>
+      <c r="R14" t="str" cm="1">
+        <f t="array" ref="R14">_xlfn.IFS($H14="", "No Data", $H14&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="28">
         <v>45117.778391203698</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="27">
         <v>70000</v>
       </c>
-      <c r="I15" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="28" t="s">
+      <c r="I15" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="27" t="s">
         <v>58</v>
       </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N15" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O15" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary Low</v>
+      </c>
+      <c r="R15" t="str" cm="1">
+        <f t="array" ref="R15">_xlfn.IFS($H15="", "No Data", $H15&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary Low</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="28">
         <v>44938.614351851851</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="27">
         <v>98301.5</v>
       </c>
-      <c r="I16" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="28" t="s">
+      <c r="I16" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="27" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N16" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O16" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary &gt; 85K</v>
+      </c>
+      <c r="R16" t="str" cm="1">
+        <f t="array" ref="R16">_xlfn.IFS($H16="", "No Data", $H16&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="28">
         <v>44985.354097222233</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="27">
         <v>89100</v>
       </c>
-      <c r="I17" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="28" t="s">
+      <c r="I17" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N17" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O17" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary &gt; 85K</v>
+      </c>
+      <c r="R17" t="str" cm="1">
+        <f t="array" ref="R17">_xlfn.IFS($H17="", "No Data", $H17&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="28">
         <v>45063.792291666658</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="G18" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" s="28" t="s">
+      <c r="H18" s="27"/>
+      <c r="I18" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="27" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N18" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O18" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q18" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary Low</v>
+      </c>
+      <c r="R18" s="45" t="str" cm="1">
+        <f t="array" ref="R18">_xlfn.IFS($H18="", "No Data", $H18&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="28">
         <v>45017.004837962973</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="28" t="s">
+      <c r="G19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H19" s="27">
         <v>87500</v>
       </c>
-      <c r="I19" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="28" t="s">
+      <c r="I19" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="27" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N19" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O19" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary &gt; 85K</v>
+      </c>
+      <c r="R19" t="str" cm="1">
+        <f t="array" ref="R19">_xlfn.IFS($H19="", "No Data", $H19&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="28">
         <v>45169.64203703704</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="G20" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" s="28" t="s">
+      <c r="H20" s="27"/>
+      <c r="I20" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" s="27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N20" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O20" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q20" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary Low</v>
+      </c>
+      <c r="R20" s="45" t="str" cm="1">
+        <f t="array" ref="R20">_xlfn.IFS($H20="", "No Data", $H20&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="28">
         <v>45000.542685185188</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21" s="27">
         <v>90000</v>
       </c>
-      <c r="I21" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="28" t="s">
+      <c r="I21" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="27" t="s">
         <v>29</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N21" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O21" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="5"/>
+        <v>Salary &gt; 85K</v>
+      </c>
+      <c r="R21" t="str" cm="1">
+        <f t="array" ref="R21">_xlfn.IFS($H21="", "No Data", $H21&gt;=Q$1, "Salary &gt; 85K", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85K</v>
       </c>
     </row>
   </sheetData>
@@ -4081,158 +4794,158 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="32" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="e">
+      <c r="B3" s="27" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="E3" s="28" t="str">
+      <c r="E3" s="27" t="str">
         <f>IFERROR(B3, "This text hides the error")</f>
         <v>This text hides the error</v>
       </c>
-      <c r="F3" s="28" t="e">
+      <c r="F3" s="27" t="e">
         <f>_xlfn.IFNA(B3, "This hides #N/A error")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="28" t="e">
+      <c r="B4" s="27" t="e">
         <f>A4 + "text"</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="28" t="str">
+      <c r="E4" s="27" t="str">
         <f t="shared" ref="E4:E9" si="0">IFERROR(B4, "This text hides the error")</f>
         <v>This text hides the error</v>
       </c>
-      <c r="F4" s="28" t="e">
+      <c r="F4" s="27" t="e">
         <f t="shared" ref="F4:F9" si="1">_xlfn.IFNA(B4, "This hides #N/A error")</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="35" t="e">
+      <c r="B5" s="34" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="28" t="str">
+      <c r="E5" s="27" t="str">
         <f t="shared" si="0"/>
         <v>This text hides the error</v>
       </c>
-      <c r="F5" s="28" t="e">
+      <c r="F5" s="27" t="e">
         <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="35" t="e" cm="1">
+      <c r="B6" s="34" t="e" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">COUNTT(A3:A9)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="E6" s="28" t="str">
+      <c r="E6" s="27" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>This text hides the error</v>
       </c>
-      <c r="F6" s="28" t="e">
+      <c r="F6" s="27" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="28" t="e">
+      <c r="B7" s="27" t="e">
         <f>VLOOKUP("Value", A1:A10, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="E7" s="28" t="str">
+      <c r="E7" s="27" t="str">
         <f t="shared" si="0"/>
         <v>This text hides the error</v>
       </c>
-      <c r="F7" s="28" t="str">
+      <c r="F7" s="27" t="str">
         <f t="shared" si="1"/>
         <v>This hides #N/A error</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="28" t="e">
+      <c r="B8" s="27" t="e">
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="28" t="str">
+      <c r="E8" s="27" t="str">
         <f t="shared" si="0"/>
         <v>This text hides the error</v>
       </c>
-      <c r="F8" s="28" t="e">
+      <c r="F8" s="27" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="28" t="e">
+      <c r="B9" s="27" t="e">
         <f>SUM(A1:A10 C1:C10)</f>
         <v>#NULL!</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="E9" s="28" t="str">
+      <c r="E9" s="27" t="str">
         <f t="shared" si="0"/>
         <v>This text hides the error</v>
       </c>
-      <c r="F9" s="28" t="e">
+      <c r="F9" s="27" t="e">
         <f t="shared" si="1"/>
         <v>#NULL!</v>
       </c>
@@ -4244,10 +4957,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2D85E7-B5C1-4D76-9510-6ECF1A373805}">
-  <dimension ref="B1:E6"/>
+  <dimension ref="B1:E18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4258,96 +4971,89 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="37" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="41" t="b">
+      <c r="B3" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="40" t="b">
         <f>AND(B3,C3)</f>
         <v>1</v>
       </c>
-      <c r="E3" s="41" t="b">
+      <c r="E3" s="40" t="b">
         <f>OR(B3,C3)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="40" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="41" t="b">
+      <c r="B4" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="40" t="b">
         <f t="shared" ref="D4:D6" si="0">AND(B4,C4)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="41" t="b">
+      <c r="E4" s="40" t="b">
         <f t="shared" ref="E4:E6" si="1">OR(B4,C4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="41" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="41" t="b">
+      <c r="B5" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="40" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="40" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="43" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="44" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="44" t="b">
+      <c r="B6" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="43" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="43" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815A64BB-E916-46AC-AE47-20DD4B54F64F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>